<commit_message>
1. Added BCA and MCA papers 2. Changed Login screen layout
</commit_message>
<xml_diff>
--- a/Nomenclature/Nomenclature for database.xlsx
+++ b/Nomenclature/Nomenclature for database.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="463">
   <si>
     <t>Country</t>
   </si>
@@ -1342,6 +1342,153 @@
   </si>
   <si>
     <t>Fundamentals of DBMS and ORACLE</t>
+  </si>
+  <si>
+    <t>BCA</t>
+  </si>
+  <si>
+    <t>Logical organization of computer</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>Programming in c</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Windows and pc software</t>
+  </si>
+  <si>
+    <t>WR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advanced programming in c </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer and programming fundamentals </t>
+  </si>
+  <si>
+    <t>CX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Office automation tools </t>
+  </si>
+  <si>
+    <t>OA</t>
+  </si>
+  <si>
+    <t>Personality development</t>
+  </si>
+  <si>
+    <t>PY</t>
+  </si>
+  <si>
+    <t>Structured system analysis and design</t>
+  </si>
+  <si>
+    <t>SX</t>
+  </si>
+  <si>
+    <t>Relational database management system</t>
+  </si>
+  <si>
+    <t>RD</t>
+  </si>
+  <si>
+    <t>Bachelors in computer administration</t>
+  </si>
+  <si>
+    <t>Masters in computer administration</t>
+  </si>
+  <si>
+    <t>MCA</t>
+  </si>
+  <si>
+    <t>Computer organization</t>
+  </si>
+  <si>
+    <t>Discrete mathematical structures</t>
+  </si>
+  <si>
+    <t>Numerical and statistical methods</t>
+  </si>
+  <si>
+    <t>Computer networks and data communication</t>
+  </si>
+  <si>
+    <t>Object oriented design using uml</t>
+  </si>
+  <si>
+    <t>Visual programming</t>
+  </si>
+  <si>
+    <t>Advanced computer architecture</t>
+  </si>
+  <si>
+    <t>Programming in java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advanced web technology </t>
+  </si>
+  <si>
+    <t>Computer architecture and parallel processing</t>
+  </si>
+  <si>
+    <t>Linux and shell programming</t>
+  </si>
+  <si>
+    <t>Principles of programming language</t>
+  </si>
+  <si>
+    <t>System programming</t>
+  </si>
+  <si>
+    <t>Web technology</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>CZ</t>
+  </si>
+  <si>
+    <t>DU</t>
+  </si>
+  <si>
+    <t>NS</t>
+  </si>
+  <si>
+    <t>VP</t>
+  </si>
+  <si>
+    <t>WT</t>
+  </si>
+  <si>
+    <t>OU</t>
+  </si>
+  <si>
+    <t>LP</t>
+  </si>
+  <si>
+    <t>PF</t>
+  </si>
+  <si>
+    <t>AW</t>
+  </si>
+  <si>
+    <t>CW</t>
+  </si>
+  <si>
+    <t>AH</t>
+  </si>
+  <si>
+    <t>PV</t>
+  </si>
+  <si>
+    <t>CQ</t>
   </si>
 </sst>
 </file>
@@ -1640,7 +1787,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1683,13 +1830,134 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2082,10 +2350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L276"/>
+  <dimension ref="A2:L329"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G246" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I257" sqref="I257"/>
+    <sheetView tabSelected="1" topLeftCell="H305" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N316" sqref="N316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2367,6 +2635,12 @@
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>432</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>205</v>
+      </c>
       <c r="H26" s="16"/>
       <c r="I26" s="16" t="s">
         <v>46</v>
@@ -2376,6 +2650,12 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>433</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="H27" s="16"/>
       <c r="I27" s="16" t="s">
         <v>47</v>
@@ -4587,7 +4867,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="273" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I273" t="s">
         <v>343</v>
       </c>
@@ -4595,7 +4875,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="274" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I274" t="s">
         <v>344</v>
       </c>
@@ -4603,7 +4883,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="275" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="275" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I275" t="s">
         <v>345</v>
       </c>
@@ -4611,7 +4891,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="276" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I276" t="s">
         <v>346</v>
       </c>
@@ -4619,38 +4899,399 @@
         <v>359</v>
       </c>
     </row>
+    <row r="277" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H277" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="278" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H278">
+        <v>1</v>
+      </c>
+      <c r="I278" t="s">
+        <v>139</v>
+      </c>
+      <c r="J278" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="279" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I279" t="s">
+        <v>415</v>
+      </c>
+      <c r="J279" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="280" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I280" t="s">
+        <v>39</v>
+      </c>
+      <c r="J280" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="281" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I281" t="s">
+        <v>417</v>
+      </c>
+      <c r="J281" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="282" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I282" t="s">
+        <v>419</v>
+      </c>
+      <c r="J282" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="283" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I283" t="s">
+        <v>421</v>
+      </c>
+      <c r="J283" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="284" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I284" t="s">
+        <v>424</v>
+      </c>
+      <c r="J284" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="285" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I285" t="s">
+        <v>426</v>
+      </c>
+      <c r="J285" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="286" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I286" t="s">
+        <v>428</v>
+      </c>
+      <c r="J286" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="287" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H287">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="288" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I288" t="s">
+        <v>430</v>
+      </c>
+      <c r="J288" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="295" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H295">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="296" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I296" t="s">
+        <v>422</v>
+      </c>
+      <c r="J296" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="297" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H297" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="298" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H298">
+        <v>1</v>
+      </c>
+      <c r="I298" t="s">
+        <v>435</v>
+      </c>
+      <c r="J298" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="299" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I299" t="s">
+        <v>436</v>
+      </c>
+      <c r="J299" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="300" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I300" t="s">
+        <v>437</v>
+      </c>
+      <c r="J300" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="301" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I301" t="s">
+        <v>417</v>
+      </c>
+      <c r="J301" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="302" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I302" t="s">
+        <v>89</v>
+      </c>
+      <c r="J302" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="303" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H303">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="304" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I304" t="s">
+        <v>448</v>
+      </c>
+      <c r="J304" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="305" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I305" t="s">
+        <v>447</v>
+      </c>
+      <c r="J305" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="306" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I306" t="s">
+        <v>446</v>
+      </c>
+      <c r="J306" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="307" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I307" t="s">
+        <v>109</v>
+      </c>
+      <c r="J307" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="308" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I308" t="s">
+        <v>122</v>
+      </c>
+      <c r="J308" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="309" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H309">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="310" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I310" t="s">
+        <v>438</v>
+      </c>
+      <c r="J310" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="311" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I311" t="s">
+        <v>117</v>
+      </c>
+      <c r="J311" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="312" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I312" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="J312" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="313" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I313" t="s">
+        <v>439</v>
+      </c>
+      <c r="J313" s="30" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="314" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I314" t="s">
+        <v>101</v>
+      </c>
+      <c r="J314" s="30" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="315" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I315" t="s">
+        <v>440</v>
+      </c>
+      <c r="J315" s="30" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="316" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H316">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="317" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I317" t="s">
+        <v>441</v>
+      </c>
+      <c r="J317" s="30" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="318" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I318" t="s">
+        <v>214</v>
+      </c>
+      <c r="J318" s="30" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="319" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I319" t="s">
+        <v>197</v>
+      </c>
+      <c r="J319" s="30" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="320" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I320" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="J320" s="30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="321" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I321" t="s">
+        <v>442</v>
+      </c>
+      <c r="J321" s="30" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="322" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H322">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="323" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I323" t="s">
+        <v>443</v>
+      </c>
+      <c r="J323" s="30" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="324" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I324" t="s">
+        <v>45</v>
+      </c>
+      <c r="J324" s="30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="325" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I325" t="s">
+        <v>60</v>
+      </c>
+      <c r="J325" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="326" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I326" t="s">
+        <v>444</v>
+      </c>
+      <c r="J326" s="30" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="327" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I327" t="s">
+        <v>197</v>
+      </c>
+      <c r="J327" s="30" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="328" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I328" t="s">
+        <v>445</v>
+      </c>
+      <c r="J328" s="30" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="329" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I329" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="J329" s="30" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="J19:J87">
-    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J88:J104">
-    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:J105">
-    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J24:J108 J110:J189 J214:J349">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  <conditionalFormatting sqref="J24:J108 J110:J189 J214:J353">
+    <cfRule type="duplicateValues" dxfId="19" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I215:I576 I24:I189">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  <conditionalFormatting sqref="I24:I189 I215:I580">
+    <cfRule type="duplicateValues" dxfId="18" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J24:J189 J214:J536">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  <conditionalFormatting sqref="J24:J189 J214:J540">
+    <cfRule type="duplicateValues" dxfId="17" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I216:J923">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  <conditionalFormatting sqref="I216:J927">
+    <cfRule type="duplicateValues" dxfId="16" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I218:I244">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J190:J213">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I190:I213">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J190:J213">
+    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24:J416">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>